<commit_message>
Fix issue of document management
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/ambient.directory.tree.xlsx
+++ b/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/ambient.directory.tree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/ox-workshop/vertx-zero/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AE56C3-E211-E348-A6B7-B2D34F8E595E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0835153-6571-9B49-84B2-47674444A531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54820" yWindow="4100" windowWidth="38400" windowHeight="16940" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="41500" yWindow="-11760" windowWidth="38400" windowHeight="16940" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-CDATA" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>code</t>
   </si>
@@ -125,6 +125,17 @@
   </si>
   <si>
     <t>ad15bf63-079f-427d-9054-12a5a5ef8522</t>
+  </si>
+  <si>
+    <t>6cdd34ca-1e4d-4e63-ba78-b0ead49a8fd2</t>
+  </si>
+  <si>
+    <t>合同管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>document.contract</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -644,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500280C7-B0AC-7C45-9420-F2551253A777}">
-  <dimension ref="A2:I6"/>
+  <dimension ref="A2:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A14" sqref="A5:XFD14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -783,6 +794,29 @@
       </c>
       <c r="I6" s="16"/>
     </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="15">
+        <v>1015</v>
+      </c>
+      <c r="I7" s="16"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:I2"/>

</xml_diff>